<commit_message>
wind power data details
</commit_message>
<xml_diff>
--- a/wind_power-data.xlsx
+++ b/wind_power-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dongenergy-my.sharepoint.com/personal/mibac_orsted_dk/Documents/Hackathon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D47C8D5-6D96-41CA-86E8-0C82CCB05774}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35DFF0F9-32C7-4E64-832A-480973757F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="19188" windowHeight="10788" xr2:uid="{58890258-4B8D-43DA-AF3F-498B3B437CE7}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="19188" windowHeight="10788" firstSheet="3" activeTab="3" xr2:uid="{58890258-4B8D-43DA-AF3F-498B3B437CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequency Table" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Area" sheetId="3" r:id="rId3"/>
     <sheet name="Test case" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
+    <t>Wind Frequency simple</t>
+  </si>
+  <si>
+    <t>Wind Frequency tables</t>
+  </si>
+  <si>
+    <t>Tabla 1a</t>
+  </si>
+  <si>
+    <t>Table 1b</t>
+  </si>
+  <si>
+    <t>Wind direction\Wind speed</t>
+  </si>
+  <si>
+    <t>Tabla 2a</t>
+  </si>
+  <si>
+    <t>Table 2b</t>
+  </si>
+  <si>
     <t>Power Curve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source: https://en.wind-turbine-models.com/turbines/1282-vestas-v136-3.45#powercurve </t>
   </si>
   <si>
     <t>wind speed</t>
@@ -45,34 +71,28 @@
     <t>Power</t>
   </si>
   <si>
-    <t xml:space="preserve">source: https://en.wind-turbine-models.com/turbines/1282-vestas-v136-3.45#powercurve </t>
-  </si>
-  <si>
-    <t>Wind Frequency tables</t>
-  </si>
-  <si>
-    <t>Wind direction\Wind speed</t>
+    <t>Cp</t>
   </si>
   <si>
     <t>Ct</t>
   </si>
   <si>
-    <t>Cp</t>
-  </si>
-  <si>
     <t>rotor dimater</t>
   </si>
   <si>
+    <t xml:space="preserve">hub height </t>
+  </si>
+  <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>Turbines</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Turbines</t>
   </si>
   <si>
     <t>TestCase</t>
@@ -84,9 +104,6 @@
     <t>windspeed turbine2</t>
   </si>
   <si>
-    <t xml:space="preserve">hub height </t>
-  </si>
-  <si>
     <t xml:space="preserve">wind direction </t>
   </si>
   <si>
@@ -95,27 +112,12 @@
   <si>
     <t>rotor diameter</t>
   </si>
-  <si>
-    <t>Wind Frequency simple</t>
-  </si>
-  <si>
-    <t>Table 1b</t>
-  </si>
-  <si>
-    <t>Tabla 1a</t>
-  </si>
-  <si>
-    <t>Tabla 2a</t>
-  </si>
-  <si>
-    <t>Table 2b</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -542,7 +544,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="341221528"/>
@@ -598,7 +600,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="341225464"/>
@@ -640,7 +642,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -677,7 +679,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1573,37 +1575,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2057559D-6D76-490E-A2E4-A1556E2EA0D7}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.15"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1684,7 +1686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>30</v>
       </c>
@@ -1774,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>60</v>
       </c>
@@ -1864,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>90</v>
       </c>
@@ -1954,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>120</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>150</v>
       </c>
@@ -2134,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>180</v>
       </c>
@@ -2224,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>210</v>
       </c>
@@ -2314,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>240</v>
       </c>
@@ -2404,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>270</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>300</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15">
         <v>330</v>
       </c>
@@ -2674,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16">
         <v>360</v>
       </c>
@@ -2764,23 +2766,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2861,7 +2863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30">
       <c r="A23">
         <v>30</v>
       </c>
@@ -2951,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30">
       <c r="A24">
         <v>60</v>
       </c>
@@ -3041,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30">
       <c r="A25">
         <v>90</v>
       </c>
@@ -3131,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30">
       <c r="A26">
         <v>120</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30">
       <c r="A27">
         <v>150</v>
       </c>
@@ -3311,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30">
       <c r="A28">
         <v>180</v>
       </c>
@@ -3401,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30">
       <c r="A29">
         <v>210</v>
       </c>
@@ -3491,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30">
       <c r="A30">
         <v>240</v>
       </c>
@@ -3581,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30">
       <c r="A31">
         <v>270</v>
       </c>
@@ -3671,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30">
       <c r="A32">
         <v>300</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30">
       <c r="A33">
         <v>330</v>
       </c>
@@ -3851,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30">
       <c r="A34">
         <v>360</v>
       </c>
@@ -3950,50 +3952,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57964E42-75AA-4447-917F-A410B50C31E5}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G24" sqref="G22:G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.15"/>
   <cols>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>136</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2.5</v>
       </c>
@@ -4008,7 +4010,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4023,7 +4025,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>3.5</v>
       </c>
@@ -4038,7 +4040,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4053,7 +4055,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>4.5</v>
       </c>
@@ -4068,7 +4070,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4083,7 +4085,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>5.5</v>
       </c>
@@ -4098,7 +4100,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>6</v>
       </c>
@@ -4113,7 +4115,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>6.5</v>
       </c>
@@ -4128,7 +4130,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>7</v>
       </c>
@@ -4143,7 +4145,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>7.5</v>
       </c>
@@ -4158,7 +4160,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>8</v>
       </c>
@@ -4173,7 +4175,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>8.5</v>
       </c>
@@ -4188,7 +4190,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>9</v>
       </c>
@@ -4203,7 +4205,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>9.5</v>
       </c>
@@ -4218,7 +4220,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>10</v>
       </c>
@@ -4233,7 +4235,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>10.5</v>
       </c>
@@ -4248,7 +4250,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>11</v>
       </c>
@@ -4263,7 +4265,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>11.5</v>
       </c>
@@ -4278,7 +4280,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>12</v>
       </c>
@@ -4293,7 +4295,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>12.5</v>
       </c>
@@ -4308,7 +4310,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>13</v>
       </c>
@@ -4323,7 +4325,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>13.5</v>
       </c>
@@ -4338,7 +4340,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>14</v>
       </c>
@@ -4353,7 +4355,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>14.5</v>
       </c>
@@ -4368,7 +4370,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>15</v>
       </c>
@@ -4383,7 +4385,7 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>15.5</v>
       </c>
@@ -4398,7 +4400,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>16</v>
       </c>
@@ -4413,7 +4415,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>16.5</v>
       </c>
@@ -4428,7 +4430,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>17</v>
       </c>
@@ -4443,7 +4445,7 @@
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>17.5</v>
       </c>
@@ -4458,7 +4460,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>18</v>
       </c>
@@ -4473,7 +4475,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>18.5</v>
       </c>
@@ -4488,7 +4490,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>19</v>
       </c>
@@ -4503,7 +4505,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>19.5</v>
       </c>
@@ -4518,7 +4520,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>20</v>
       </c>
@@ -4533,7 +4535,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>20.5</v>
       </c>
@@ -4548,7 +4550,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>21</v>
       </c>
@@ -4563,7 +4565,7 @@
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>21.5</v>
       </c>
@@ -4578,7 +4580,7 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>22</v>
       </c>
@@ -4593,7 +4595,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>22.5</v>
       </c>
@@ -4608,7 +4610,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>23</v>
       </c>
@@ -4633,35 +4635,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5F9390-85E5-4421-AD3E-F53889EEF4D9}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4675,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>11000</v>
       </c>
@@ -4689,7 +4691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>12000</v>
       </c>
@@ -4703,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -4717,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5000</v>
       </c>
@@ -4731,7 +4733,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>3000</v>
       </c>
@@ -4745,7 +4747,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>3000</v>
       </c>
@@ -4759,7 +4761,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>0</v>
       </c>
@@ -4773,7 +4775,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>0</v>
       </c>
@@ -4787,7 +4789,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="D12">
         <v>1300</v>
       </c>
@@ -4795,7 +4797,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="D13">
         <v>2600</v>
       </c>
@@ -4803,7 +4805,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="D14">
         <v>3900</v>
       </c>
@@ -4811,7 +4813,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="D15">
         <v>0</v>
       </c>
@@ -4819,7 +4821,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="D16">
         <v>1300</v>
       </c>
@@ -4827,7 +4829,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5">
       <c r="D17">
         <v>2600</v>
       </c>
@@ -4835,7 +4837,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5">
       <c r="D18">
         <v>3900</v>
       </c>
@@ -4843,7 +4845,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5">
       <c r="D19">
         <v>0</v>
       </c>
@@ -4851,7 +4853,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:5">
       <c r="D20">
         <v>1300</v>
       </c>
@@ -4859,7 +4861,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:5">
       <c r="D21">
         <v>2600</v>
       </c>
@@ -4867,7 +4869,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:5">
       <c r="D22">
         <v>3900</v>
       </c>
@@ -4875,7 +4877,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5">
       <c r="D23">
         <v>0</v>
       </c>
@@ -4883,7 +4885,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:5">
       <c r="D24">
         <v>1300</v>
       </c>
@@ -4891,7 +4893,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:5">
       <c r="D25">
         <v>2600</v>
       </c>
@@ -4899,7 +4901,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:5">
       <c r="D26">
         <v>3900</v>
       </c>
@@ -4917,41 +4919,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E014CA6-7DEE-4365-A64A-1C9F456BC03F}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2.5</v>
       </c>
@@ -4974,7 +4976,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4989,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>3.5</v>
       </c>
@@ -4997,7 +4999,7 @@
         <v>2.23269346614252</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5005,7 +5007,7 @@
         <v>2.5219805554853099</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>4.5</v>
       </c>
@@ -5013,7 +5015,7 @@
         <v>2.8372281249209701</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>5</v>
       </c>
@@ -5021,7 +5023,7 @@
         <v>3.1143998023772999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>5.5</v>
       </c>
@@ -5029,7 +5031,7 @@
         <v>3.4258397826150402</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5037,7 +5039,7 @@
         <v>3.6903008636718102</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>6.5</v>
       </c>
@@ -5045,7 +5047,7 @@
         <v>3.9978259356444599</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>7</v>
       </c>
@@ -5053,7 +5055,7 @@
         <v>4.3053510076171104</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>7.5</v>
       </c>
@@ -5061,7 +5063,7 @@
         <v>4.6715997035659598</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>8</v>
       </c>
@@ -5069,7 +5071,7 @@
         <v>4.9830396838036899</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>8.5</v>
       </c>
@@ -5077,7 +5079,7 @@
         <v>5.3592086804062804</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>9</v>
       </c>
@@ -5085,7 +5087,7 @@
         <v>5.8698921524126</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>9.5</v>
       </c>
@@ -5093,7 +5095,7 @@
         <v>6.4502597257088796</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>10</v>
       </c>
@@ -5101,7 +5103,7 @@
         <v>7.0374805927412698</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>10.5</v>
       </c>
@@ -5109,7 +5111,7 @@
         <v>7.6911870122901496</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>11</v>
       </c>
@@ -5117,7 +5119,7 @@
         <v>8.3517507866146001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>11.5</v>
       </c>
@@ -5125,7 +5127,7 @@
         <v>9.0203691050669708</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>12</v>
       </c>
@@ -5133,7 +5135,7 @@
         <v>9.7530852626832107</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>12.5</v>
       </c>
@@ -5141,7 +5143,7 @@
         <v>10.4938577644765</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>13</v>
       </c>
@@ -5149,7 +5151,7 @@
         <v>11.135363299281201</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>13.5</v>
       </c>
@@ -5157,7 +5159,7 @@
         <v>11.786492325682399</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>14</v>
       </c>
@@ -5165,7 +5167,7 @@
         <v>12.447120533115701</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>14.5</v>
       </c>
@@ -5173,7 +5175,7 @@
         <v>13.0613463749437</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>15</v>
       </c>
@@ -5181,7 +5183,7 @@
         <v>13.6836541995809</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>15.5</v>
       </c>
@@ -5189,7 +5191,7 @@
         <v>14.2562397047224</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>16</v>
       </c>
@@ -5197,7 +5199,7 @@
         <v>14.8347875683979</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>16.5</v>
       </c>
@@ -5205,7 +5207,7 @@
         <v>15.419212730351299</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>17</v>
       </c>
@@ -5213,7 +5215,7 @@
         <v>15.9481350790197</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>17.5</v>
       </c>
@@ -5221,7 +5223,7 @@
         <v>16.543021780443699</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>18</v>
       </c>
@@ -5229,7 +5231,7 @@
         <v>17.079811183544098</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>18.5</v>
       </c>
@@ -5237,7 +5239,7 @@
         <v>17.6197768584809</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>19</v>
       </c>
@@ -5245,7 +5247,7 @@
         <v>18.162894364988301</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>19.5</v>
       </c>
@@ -5253,7 +5255,7 @@
         <v>18.709139786605999</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>20</v>
       </c>
@@ -5261,7 +5263,7 @@
         <v>19.258489712904002</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>20.5</v>
       </c>
@@ -5269,7 +5271,7 @@
         <v>19.810921222520701</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>21</v>
       </c>
@@ -5277,7 +5279,7 @@
         <v>20.366411866965599</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>21.5</v>
       </c>
@@ -5285,7 +5287,7 @@
         <v>20.851326435226699</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>22</v>
       </c>
@@ -5293,7 +5295,7 @@
         <v>21.3362410034878</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>22.5</v>
       </c>
@@ -5301,7 +5303,7 @@
         <v>21.898192662362199</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>23</v>
       </c>
@@ -5315,21 +5317,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A7CAE3CFA1DCBA428783EF3795C4DA52" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c023da8cd2233c25f61b36ac627cd4c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1830ec8-ece2-412b-8c34-3ea12cf663f0" xmlns:ns4="6872e9fd-68ad-461c-860c-26817f127035" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23e19cbb8212eee5e1d8d504d395172b" ns3:_="" ns4:_="">
     <xsd:import namespace="a1830ec8-ece2-412b-8c34-3ea12cf663f0"/>
@@ -5520,46 +5507,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DA4688-B069-4307-9CF5-F7212FB99B54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="a1830ec8-ece2-412b-8c34-3ea12cf663f0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6872e9fd-68ad-461c-860c-26817f127035"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E29E959C-FBB1-4B22-9AA5-3A1C449C01CB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541D913D-F0B5-4817-B8E6-75E3538295D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541D913D-F0B5-4817-B8E6-75E3538295D7}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E29E959C-FBB1-4B22-9AA5-3A1C449C01CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1830ec8-ece2-412b-8c34-3ea12cf663f0"/>
-    <ds:schemaRef ds:uri="6872e9fd-68ad-461c-860c-26817f127035"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DA4688-B069-4307-9CF5-F7212FB99B54}"/>
 </file>
</xml_diff>